<commit_message>
TP1 & 2 WIP
</commit_message>
<xml_diff>
--- a/prez/data/afrika.xlsx
+++ b/prez/data/afrika.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
@@ -500,7 +500,7 @@
     <t xml:space="preserve">Definition</t>
   </si>
   <si>
-    <t xml:space="preserve">Souce</t>
+    <t xml:space="preserve">Source</t>
   </si>
   <si>
     <t xml:space="preserve">ISO3 code of country</t>
@@ -683,18 +683,18 @@
   </sheetPr>
   <dimension ref="A1:Z50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y24" activeCellId="0" sqref="Y24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="25.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="9" style="0" width="7.95"/>
@@ -4720,11 +4720,11 @@
   </sheetPr>
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E27" activeCellId="0" sqref="E27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="14.65" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="62.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="37.76"/>

</xml_diff>